<commit_message>
Updates on domain design and sprint backlog
</commit_message>
<xml_diff>
--- a/documents/Deliverable_4/FlyingMongeese_Deliverable_4_SprintBacklog.xlsx
+++ b/documents/Deliverable_4/FlyingMongeese_Deliverable_4_SprintBacklog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cadew\OneDrive\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur Bhakta\Documents\GitHub\Software2project\documents\Deliverable_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF31828-4947-4769-B425-94F0B689A0CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B031B9E4-B4C3-454D-B165-79314CAD0C15}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="450" windowWidth="22740" windowHeight="15570" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1872" yWindow="456" windowWidth="22740" windowHeight="15576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SprintBacklog1" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="SprintBacklog3" sheetId="4" r:id="rId3"/>
     <sheet name="SprintBacklog4" sheetId="5" r:id="rId4"/>
     <sheet name="SprintBacklog5" sheetId="6" r:id="rId5"/>
+    <sheet name="SprintBacklog6" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="129">
   <si>
     <t>Story Type</t>
   </si>
@@ -668,6 +669,34 @@
 Turner:X
 Mayur:X
 Riggs:
+Carolyn:</t>
+  </si>
+  <si>
+    <t>Week 1(04/30/2018)</t>
+  </si>
+  <si>
+    <t>Week 2(05/07/2018)</t>
+  </si>
+  <si>
+    <t>Cade:X
+Andre:
+Turner:
+Mayur:X
+Riggs:
+Carolyn:</t>
+  </si>
+  <si>
+    <t>Start planning on how calculate specific sales margins based on sales prediction.</t>
+  </si>
+  <si>
+    <t>Expand upload sales data for one day method so the user can upload past days or year sales data.</t>
+  </si>
+  <si>
+    <t>Cade: X
+Andre:
+Turner:
+Mayur:
+Riggs: X
 Carolyn:</t>
   </si>
 </sst>
@@ -892,14 +921,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,7 +944,15 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1272,24 +1309,24 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1315,7 +1352,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>10</v>
       </c>
@@ -1338,7 +1375,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>11</v>
       </c>
@@ -1361,7 +1398,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>12</v>
       </c>
@@ -1384,7 +1421,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>13</v>
       </c>
@@ -1407,7 +1444,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>14</v>
       </c>
@@ -1430,7 +1467,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>15</v>
       </c>
@@ -1455,7 +1492,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>16</v>
       </c>
@@ -1480,7 +1517,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>17</v>
       </c>
@@ -1505,7 +1542,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>18</v>
       </c>
@@ -1528,7 +1565,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>19</v>
       </c>
@@ -1551,7 +1588,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>20</v>
       </c>
@@ -1576,12 +1613,12 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="9" t="s">
         <v>31</v>
@@ -1592,7 +1629,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="9" t="s">
         <v>32</v>
@@ -1609,7 +1646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="9" t="s">
         <v>33</v>
@@ -1626,7 +1663,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="9" t="s">
         <v>34</v>
@@ -1643,7 +1680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="9" t="s">
         <v>38</v>
@@ -1660,7 +1697,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="9" t="s">
         <v>39</v>
@@ -1677,7 +1714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="9" t="s">
         <v>40</v>
@@ -1694,7 +1731,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>46</v>
       </c>
@@ -1708,10 +1745,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
     </row>
   </sheetData>
@@ -1720,7 +1757,7 @@
     <mergeCell ref="A14:XFD14"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1736,19 +1773,19 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="7" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:11" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>12</v>
       </c>
@@ -1774,7 +1811,7 @@
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
     </row>
-    <row r="3" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A3" s="23">
         <v>10</v>
       </c>
@@ -1799,7 +1836,7 @@
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
     </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A4" s="23">
         <v>11</v>
       </c>
@@ -1824,7 +1861,7 @@
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
     </row>
-    <row r="5" spans="1:11" s="12" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="12" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A5" s="23">
         <v>12</v>
       </c>
@@ -1847,7 +1884,7 @@
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A6" s="23">
         <v>13</v>
       </c>
@@ -1870,7 +1907,7 @@
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
     </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="12" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A7" s="23">
         <v>14</v>
       </c>
@@ -1893,7 +1930,7 @@
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:11" s="12" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="12" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <v>15</v>
       </c>
@@ -1918,7 +1955,7 @@
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>16</v>
       </c>
@@ -1943,7 +1980,7 @@
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>17</v>
       </c>
@@ -1968,7 +2005,7 @@
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <v>18</v>
       </c>
@@ -1991,7 +2028,7 @@
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>20</v>
       </c>
@@ -2016,12 +2053,12 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:11" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
+    <row r="13" spans="1:11" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="B14" s="38" t="s">
         <v>31</v>
@@ -2036,13 +2073,13 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="23"/>
       <c r="F15" s="26" t="s">
         <v>75</v>
@@ -2051,13 +2088,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="23"/>
       <c r="F16" s="26" t="s">
         <v>4</v>
@@ -2066,13 +2103,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="18" t="s">
         <v>49</v>
       </c>
@@ -2083,13 +2120,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
       <c r="E18" s="23"/>
       <c r="F18" s="26" t="s">
         <v>4</v>
@@ -2098,13 +2135,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="27" t="s">
         <v>44</v>
       </c>
@@ -2115,13 +2152,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="23"/>
       <c r="F20" s="26" t="s">
         <v>4</v>
@@ -2130,13 +2167,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="23"/>
       <c r="F21" s="26" t="s">
         <v>4</v>
@@ -2145,13 +2182,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="23"/>
       <c r="F22" s="26" t="s">
         <v>4</v>
@@ -2160,13 +2197,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="23" t="s">
         <v>48</v>
       </c>
@@ -2179,21 +2216,21 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A13:XFD13"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2210,22 +2247,22 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
     <col min="6" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:7" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -2248,7 +2285,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>10</v>
       </c>
@@ -2267,7 +2304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>11</v>
       </c>
@@ -2286,7 +2323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>12</v>
       </c>
@@ -2305,7 +2342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>13</v>
       </c>
@@ -2324,7 +2361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>14</v>
       </c>
@@ -2343,7 +2380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>15</v>
       </c>
@@ -2362,7 +2399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>16</v>
       </c>
@@ -2381,7 +2418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>17</v>
       </c>
@@ -2400,7 +2437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>18</v>
       </c>
@@ -2419,7 +2456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>19</v>
       </c>
@@ -2438,7 +2475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>20</v>
       </c>
@@ -2457,23 +2494,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+    <row r="14" spans="1:7" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-    </row>
-    <row r="16" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+    </row>
+    <row r="16" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="38" t="s">
         <v>32</v>
@@ -2490,7 +2527,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="38" t="s">
         <v>33</v>
@@ -2507,7 +2544,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="38" t="s">
         <v>61</v>
@@ -2524,7 +2561,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="38" t="s">
         <v>38</v>
@@ -2541,7 +2578,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="38" t="s">
         <v>39</v>
@@ -2558,7 +2595,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
       <c r="B21" s="38" t="s">
         <v>35</v>
@@ -2575,7 +2612,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="38" t="s">
         <v>37</v>
@@ -2592,7 +2629,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
       <c r="B23" s="38" t="s">
         <v>36</v>
@@ -2609,7 +2646,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="38" t="s">
         <v>40</v>
@@ -2626,16 +2663,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:XFD1"/>
+    <mergeCell ref="A14:XFD14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B24:D24"/>
@@ -2643,14 +2685,9 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="A1:XFD1"/>
-    <mergeCell ref="A14:XFD14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2663,26 +2700,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" style="3" customWidth="1"/>
     <col min="6" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:7" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -2705,7 +2742,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>10</v>
       </c>
@@ -2726,7 +2763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>11</v>
       </c>
@@ -2747,7 +2784,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="12" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>12</v>
       </c>
@@ -2768,7 +2805,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>13</v>
       </c>
@@ -2787,7 +2824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>14</v>
       </c>
@@ -2806,7 +2843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>15</v>
       </c>
@@ -2827,7 +2864,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>16</v>
       </c>
@@ -2848,7 +2885,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>17</v>
       </c>
@@ -2869,7 +2906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>18</v>
       </c>
@@ -2890,7 +2927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>19</v>
       </c>
@@ -2909,7 +2946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>20</v>
       </c>
@@ -2928,7 +2965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>21</v>
       </c>
@@ -2947,26 +2984,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:7" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+    <row r="16" spans="1:7" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-    </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+    </row>
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="38" t="s">
         <v>32</v>
@@ -2983,7 +3020,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="38" t="s">
         <v>33</v>
@@ -3000,7 +3037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="38" t="s">
         <v>61</v>
@@ -3017,7 +3054,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
       <c r="B21" s="38" t="s">
         <v>38</v>
@@ -3034,7 +3071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="38" t="s">
         <v>39</v>
@@ -3051,7 +3088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
       <c r="B23" s="38" t="s">
         <v>35</v>
@@ -3068,7 +3105,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="38" t="s">
         <v>37</v>
@@ -3085,7 +3122,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
       <c r="B25" s="38" t="s">
         <v>36</v>
@@ -3102,7 +3139,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A26" s="20"/>
       <c r="B26" s="38" t="s">
         <v>40</v>
@@ -3119,7 +3156,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
         <v>114</v>
       </c>
@@ -3135,7 +3172,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28"/>
     </row>
   </sheetData>
@@ -3155,7 +3192,7 @@
     <mergeCell ref="B25:D25"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3168,26 +3205,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
     <col min="6" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:7" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -3210,7 +3247,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>10</v>
       </c>
@@ -3231,7 +3268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>11</v>
       </c>
@@ -3252,7 +3289,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="12" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>12</v>
       </c>
@@ -3273,7 +3310,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>13</v>
       </c>
@@ -3292,7 +3329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>14</v>
       </c>
@@ -3311,7 +3348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>15</v>
       </c>
@@ -3332,7 +3369,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>16</v>
       </c>
@@ -3353,7 +3390,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>17</v>
       </c>
@@ -3374,7 +3411,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>18</v>
       </c>
@@ -3395,7 +3432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>19</v>
       </c>
@@ -3414,7 +3451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>20</v>
       </c>
@@ -3433,7 +3470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
         <v>84</v>
@@ -3448,23 +3485,23 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+    <row r="15" spans="1:7" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-    </row>
-    <row r="17" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+    </row>
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="38" t="s">
         <v>32</v>
@@ -3481,7 +3518,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="38" t="s">
         <v>33</v>
@@ -3498,7 +3535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="38" t="s">
         <v>61</v>
@@ -3515,7 +3552,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="38" t="s">
         <v>38</v>
@@ -3532,7 +3569,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
       <c r="B21" s="38" t="s">
         <v>39</v>
@@ -3549,7 +3586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
       <c r="B22" s="38" t="s">
         <v>35</v>
@@ -3566,7 +3603,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
       <c r="B23" s="38" t="s">
         <v>71</v>
@@ -3583,7 +3620,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
       <c r="B24" s="38" t="s">
         <v>36</v>
@@ -3600,7 +3637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
       <c r="B25" s="38" t="s">
         <v>40</v>
@@ -3617,7 +3654,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="38" t="s">
         <v>87</v>
@@ -3634,7 +3671,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
         <v>114</v>
       </c>
@@ -3650,7 +3687,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
       <c r="B28" s="38" t="s">
         <v>119</v>
       </c>
@@ -3685,6 +3722,525 @@
     <mergeCell ref="B24:D24"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7A854D-36D4-4862-A322-F95941A93F31}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="37.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="35" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>10</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>11</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>12</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>13</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>14</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
+        <v>15</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
+        <v>16</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>17</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>18</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>19</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>20</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
+      <c r="B16" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+    </row>
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="20"/>
+      <c r="B24" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="20"/>
+      <c r="B25" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
+      <c r="B27" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
+      <c r="B28" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A1:XFD1"/>
+    <mergeCell ref="A15:XFD15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A2:B2">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>

</xml_diff>